<commit_message>
Fix issue with address in Patient profiles
Also remove US Core dependency and bump to v0.2.1
</commit_message>
<xml_diff>
--- a/input/images/data-dictionary/data_dictionary.xlsx
+++ b/input/images/data-dictionary/data_dictionary.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82CEF4A0-81D9-1B4F-B026-B38AF7E6D755}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB3CE8C1-7E9B-E849-911C-B115B8034676}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="57600" windowHeight="31940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="57600" windowHeight="31940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IG information" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="228">
   <si>
     <t/>
   </si>
@@ -53,7 +53,7 @@
     <t>IG version</t>
   </si>
   <si>
-    <t>0.2.0</t>
+    <t>0.2.1</t>
   </si>
   <si>
     <t>FHIR version</t>
@@ -65,7 +65,7 @@
     <t>Date generated</t>
   </si>
   <si>
-    <t>3/4/2021, 5:29:17 PM</t>
+    <t>3/5/2021, 5:49:01 PM</t>
   </si>
   <si>
     <t># Profiles</t>
@@ -510,6 +510,27 @@
   </si>
   <si>
     <t>Patient.birthDate</t>
+  </si>
+  <si>
+    <t>Address &gt; Postal Code</t>
+  </si>
+  <si>
+    <t>A postal code designating a region defined by the postal service.</t>
+  </si>
+  <si>
+    <t>Required if known (conditional on Address)</t>
+  </si>
+  <si>
+    <t>Patient.address.postalCode</t>
+  </si>
+  <si>
+    <t>Address &gt; Country</t>
+  </si>
+  <si>
+    <t>Country - a nation as commonly understood or generally accepted.</t>
+  </si>
+  <si>
+    <t>Patient.address.country</t>
   </si>
   <si>
     <t>Reference to a VaccineCredentialPatient-conforming resource who had a reaction to the vaccine.</t>
@@ -720,25 +741,21 @@
       <b/>
       <sz val="11"/>
       <name val="Helvetica"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Helvetica"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
       <name val="Helvetica"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Helvetica"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -843,8 +860,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="profile_data_elements" displayName="profile_data_elements" ref="A1:L59">
-  <autoFilter ref="A1:L59" xr:uid="{00000000-0009-0000-0100-000002000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="profile_data_elements" displayName="profile_data_elements" ref="A1:L63">
+  <autoFilter ref="A1:L63" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="1">
       <filters>
         <filter val="COVID-19 Laboratory Result Observation Profile - Allowable Data"/>
@@ -1225,7 +1242,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView zoomScale="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2547,22 +2564,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L60"/>
+  <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0">
+    <sheetView zoomScale="130" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" style="1" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="58" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="1" customWidth="1"/>
     <col min="4" max="4" width="75" style="3" customWidth="1"/>
-    <col min="5" max="5" width="40" style="1" customWidth="1"/>
+    <col min="5" max="5" width="42" style="1" customWidth="1"/>
     <col min="6" max="6" width="19" style="1" customWidth="1"/>
     <col min="7" max="8" width="30" style="3" customWidth="1"/>
     <col min="9" max="9" width="17" style="1" customWidth="1"/>
@@ -4394,27 +4411,27 @@
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="1:12" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" s="14" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>69</v>
+        <v>160</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="G49" s="16" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="H49" s="16" t="s">
         <v>0</v>
@@ -4423,30 +4440,30 @@
         <v>0</v>
       </c>
       <c r="J49" s="15" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
       <c r="K49" s="15" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L49" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" s="14" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" s="14" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>144</v>
+        <v>163</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="F50" s="15" t="s">
         <v>70</v>
@@ -4461,13 +4478,13 @@
         <v>0</v>
       </c>
       <c r="J50" s="15" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
       <c r="K50" s="15" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L50" s="15" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:12" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -4478,19 +4495,19 @@
         <v>38</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>145</v>
+        <v>69</v>
       </c>
       <c r="F51" s="15" t="s">
         <v>104</v>
       </c>
       <c r="G51" s="16" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="H51" s="16" t="s">
         <v>0</v>
@@ -4499,7 +4516,7 @@
         <v>0</v>
       </c>
       <c r="J51" s="15" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="K51" s="15" t="s">
         <v>39</v>
@@ -4516,28 +4533,28 @@
         <v>38</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>86</v>
+        <v>145</v>
       </c>
       <c r="F52" s="15" t="s">
         <v>70</v>
       </c>
       <c r="G52" s="16" t="s">
-        <v>71</v>
+        <v>128</v>
       </c>
       <c r="H52" s="16" t="s">
-        <v>152</v>
+        <v>0</v>
       </c>
       <c r="I52" s="15" t="s">
-        <v>73</v>
+        <v>0</v>
       </c>
       <c r="J52" s="15" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="K52" s="15" t="s">
         <v>39</v>
@@ -4554,19 +4571,19 @@
         <v>38</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D53" s="16" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E53" s="15" t="s">
-        <v>86</v>
+        <v>145</v>
       </c>
       <c r="F53" s="15" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="G53" s="16" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="H53" s="16" t="s">
         <v>0</v>
@@ -4575,7 +4592,7 @@
         <v>0</v>
       </c>
       <c r="J53" s="15" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="K53" s="15" t="s">
         <v>39</v>
@@ -4584,141 +4601,141 @@
         <v>39</v>
       </c>
     </row>
-    <row r="54" spans="1:12" s="14" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" s="14" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E54" s="15" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="F54" s="15" t="s">
         <v>70</v>
       </c>
       <c r="G54" s="16" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="H54" s="16" t="s">
-        <v>0</v>
+        <v>152</v>
       </c>
       <c r="I54" s="15" t="s">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="J54" s="15" t="s">
-        <v>83</v>
+        <v>153</v>
       </c>
       <c r="K54" s="15" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="L54" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" s="14" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C55" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="D55" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="E55" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="F55" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="G55" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="H55" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="I55" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="J55" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="K55" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="L55" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C56" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="D56" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="D55" s="16" t="s">
+      <c r="E56" s="15" t="s">
         <v>160</v>
-      </c>
-      <c r="E55" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="F55" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="G55" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="H55" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="I55" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="J55" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="K55" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="L55" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" s="14" customFormat="1" ht="64" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B56" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C56" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="D56" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E56" s="15" t="s">
-        <v>69</v>
       </c>
       <c r="F56" s="15" t="s">
         <v>70</v>
       </c>
       <c r="G56" s="16" t="s">
-        <v>77</v>
+        <v>128</v>
       </c>
       <c r="H56" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="I56" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="J56" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="K56" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="L56" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C57" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D57" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="I56" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="J56" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="K56" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="L56" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" s="14" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A57" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B57" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C57" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="D57" s="16" t="s">
-        <v>158</v>
-      </c>
       <c r="E57" s="15" t="s">
-        <v>69</v>
+        <v>160</v>
       </c>
       <c r="F57" s="15" t="s">
         <v>70</v>
       </c>
       <c r="G57" s="16" t="s">
-        <v>82</v>
+        <v>128</v>
       </c>
       <c r="H57" s="16" t="s">
         <v>0</v>
@@ -4727,36 +4744,36 @@
         <v>0</v>
       </c>
       <c r="J57" s="15" t="s">
-        <v>83</v>
+        <v>164</v>
       </c>
       <c r="K57" s="15" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="L57" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" s="14" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" s="14" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>159</v>
+        <v>80</v>
       </c>
       <c r="D58" s="16" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="E58" s="15" t="s">
         <v>69</v>
       </c>
       <c r="F58" s="15" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="G58" s="16" t="s">
-        <v>161</v>
+        <v>82</v>
       </c>
       <c r="H58" s="16" t="s">
         <v>0</v>
@@ -4765,54 +4782,206 @@
         <v>0</v>
       </c>
       <c r="J58" s="15" t="s">
-        <v>162</v>
+        <v>83</v>
       </c>
       <c r="K58" s="15" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="L58" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" s="14" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" s="14" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>93</v>
+        <v>166</v>
       </c>
       <c r="D59" s="16" t="s">
-        <v>94</v>
+        <v>167</v>
       </c>
       <c r="E59" s="15" t="s">
         <v>69</v>
       </c>
       <c r="F59" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="G59" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="H59" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="I59" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="J59" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="K59" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="L59" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" s="14" customFormat="1" ht="64" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D60" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E60" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F60" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="G59" s="16" t="s">
+      <c r="G60" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="H59" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="I59" s="15" t="s">
+      <c r="H60" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="I60" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="J59" s="15" t="s">
+      <c r="J60" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="K59" s="15" t="s">
+      <c r="K60" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="L60" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" s="14" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A61" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B61" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D61" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="E61" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F61" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="G61" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="H61" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="I61" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="J61" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="K61" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="L59" s="15" t="s">
+      <c r="L61" s="15" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="60" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="1:12" s="14" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A62" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B62" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C62" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="D62" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="E62" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F62" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="G62" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="H62" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="I62" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="J62" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="K62" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="L62" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" s="14" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A63" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B63" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C63" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D63" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E63" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F63" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="G63" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="H63" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="I63" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="J63" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="K63" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="L63" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
@@ -4848,123 +5017,123 @@
     </row>
     <row r="2" spans="1:3" s="14" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>78</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="14" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>96</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="14" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>120</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -4993,24 +5162,24 @@
   <sheetData>
     <row r="1" spans="1:5" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>75</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="17" customFormat="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="18"/>
@@ -5019,109 +5188,109 @@
     </row>
     <row r="3" spans="1:5" s="14" customFormat="1" ht="16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="14" customFormat="1" ht="16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="14" customFormat="1" ht="16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="14" customFormat="1" ht="16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="14" customFormat="1" ht="16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="14" customFormat="1" ht="16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="17" customFormat="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="18"/>
@@ -5130,41 +5299,41 @@
     </row>
     <row r="10" spans="1:5" s="14" customFormat="1" ht="16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="14" customFormat="1" ht="16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="17" customFormat="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="18"/>
@@ -5173,16 +5342,16 @@
     </row>
     <row r="13" spans="1:5" s="14" customFormat="1" ht="16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="E13" s="16" t="s">
         <v>0</v>
@@ -5190,16 +5359,16 @@
     </row>
     <row r="14" spans="1:5" s="14" customFormat="1" ht="16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="E14" s="16" t="s">
         <v>0</v>
@@ -5207,16 +5376,16 @@
     </row>
     <row r="15" spans="1:5" s="14" customFormat="1" ht="16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="E15" s="16" t="s">
         <v>0</v>
@@ -5224,16 +5393,16 @@
     </row>
     <row r="16" spans="1:5" s="14" customFormat="1" ht="16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="E16" s="16" t="s">
         <v>0</v>
@@ -5241,7 +5410,7 @@
     </row>
     <row r="17" spans="1:5" s="17" customFormat="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="18"/>
@@ -5250,13 +5419,13 @@
     </row>
     <row r="18" spans="1:5" s="14" customFormat="1" ht="16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>0</v>

</xml_diff>